<commit_message>
chrome and chrome mobile fixes
</commit_message>
<xml_diff>
--- a/nissan/src/test/resources/datasheets/BrowserProfiles.xlsx
+++ b/nissan/src/test/resources/datasheets/BrowserProfiles.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25620" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="browserProfiles" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Browser Profile</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>ChromeWeb</t>
   </si>
 </sst>
 </file>
@@ -90,8 +93,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -115,19 +128,29 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -490,14 +513,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Psyma close and multy browser for pages availability test
</commit_message>
<xml_diff>
--- a/nissan/src/test/resources/datasheets/BrowserProfiles.xlsx
+++ b/nissan/src/test/resources/datasheets/BrowserProfiles.xlsx
@@ -93,8 +93,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -128,7 +132,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -140,6 +144,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -151,6 +157,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -483,7 +491,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -518,18 +526,18 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>